<commit_message>
Time tracking and updated readme with explanation about decisions taken
</commit_message>
<xml_diff>
--- a/docs/Work time tracking.xlsx
+++ b/docs/Work time tracking.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/144920e1c9f50389/TB/MineSweeper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{5513BF9E-31F5-4CE7-B553-5E70F94B2980}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D0997B73-39B2-4E15-94BD-15827A647E0F}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{5513BF9E-31F5-4CE7-B553-5E70F94B2980}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{58A2EC75-C09E-4ED7-A2B4-2A62F8FC65ED}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C1E058A-3A97-4062-A468-7B6413BF2A3E}"/>
+    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{0C1E058A-3A97-4062-A468-7B6413BF2A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Day</t>
   </si>
@@ -71,6 +70,42 @@
   </si>
   <si>
     <t>Game basic validation. Started visit cell endpoint</t>
+  </si>
+  <si>
+    <t>Visit cell endpoint. Calculate cell value on game creation.</t>
+  </si>
+  <si>
+    <t>Finished visit cell endpoint functionally.</t>
+  </si>
+  <si>
+    <t>NodeJS structure for api client lib.</t>
+  </si>
+  <si>
+    <t>Methods to create a game and visit a cell on client api.</t>
+  </si>
+  <si>
+    <t>Endpoint to flag a cell.</t>
+  </si>
+  <si>
+    <t>Endpoints to pause/resume a game.</t>
+  </si>
+  <si>
+    <t>Game time tracking.</t>
+  </si>
+  <si>
+    <t>Methods to pause, resume, get a game and method to flag a cell on client api.</t>
+  </si>
+  <si>
+    <t>Endpoints to create user and login.</t>
+  </si>
+  <si>
+    <t>Added swagger documentation and authorization on API.</t>
+  </si>
+  <si>
+    <t>Added methods to create user and login on client api.</t>
+  </si>
+  <si>
+    <t>Deploy configuration.</t>
   </si>
 </sst>
 </file>
@@ -79,9 +114,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh:mm"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,19 +132,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -139,16 +174,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,27 +501,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B63A8C-9396-4DDC-A977-A3EDA46E6689}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" customWidth="1"/>
+    <col min="4" max="4" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="4">
         <f>SUM(E4:E27)</f>
-        <v>0.34444444444444444</v>
-      </c>
+        <v>0.88194444444444453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -508,10 +551,10 @@
       <c r="A4" s="2">
         <v>44332</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>2.8472222222222222E-2</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -526,10 +569,10 @@
       <c r="A5" s="2">
         <v>44332</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.65277777777777779</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.72916666666666663</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -544,10 +587,10 @@
       <c r="A6" s="2">
         <v>44332</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.76388888888888884</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.79166666666666663</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -562,10 +605,10 @@
       <c r="A7" s="2">
         <v>44332</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.91666666666666663</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -580,10 +623,10 @@
       <c r="A8" s="2">
         <v>44332</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.97916666666666663</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -598,10 +641,10 @@
       <c r="A9" s="2">
         <v>44333</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>3.8194444444444441E-2</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -613,149 +656,261 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="2">
+        <v>44333</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
+        <v>2.7083333333333348E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>44334</v>
+      </c>
+      <c r="B11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="5">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>44334</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.9375</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>44334</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.98263888888888884</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666718E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>44335</v>
+      </c>
+      <c r="B14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="5">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="2">
+        <v>44335</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.89930555555555547</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.94652777777777775</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.7222222222222276E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="2">
+        <v>44335</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.94652777777777775</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5694444444444464E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="1"/>
+      <c r="A17" s="2">
+        <v>44335</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.97569444444444453</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.98819444444444438</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.2499999999999845E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="1"/>
+      <c r="A18" s="2">
+        <v>44336</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.0555555555555555E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="1"/>
+      <c r="A19" s="2">
+        <v>44336</v>
+      </c>
+      <c r="B19" s="5">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.2222222222222213E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="1"/>
+      <c r="A20" s="2">
+        <v>44338</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.10138888888888892</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="2">
+        <v>44338</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="E21" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="1"/>
+      <c r="A22" s="2">
+        <v>44338</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E22" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.777777777777779E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="2">
+        <v>44339</v>
+      </c>
+      <c r="B23" s="5">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C23" s="5">
+        <v>5.6250000000000001E-2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E23" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.9305555555555561E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="1"/>
       <c r="E24" s="3">
         <f t="shared" si="0"/>
@@ -764,8 +919,8 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="1"/>
       <c r="E25" s="3">
         <f t="shared" si="0"/>
@@ -774,8 +929,8 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="1"/>
       <c r="E26" s="3">
         <f t="shared" si="0"/>
@@ -784,8 +939,8 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="1"/>
       <c r="E27" s="3">
         <f t="shared" si="0"/>
@@ -799,19 +954,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D9F8D0-8880-4D7F-8BCB-B464ABFDD71D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:N16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>